<commit_message>
Updates to input descriptions, download files, and data table 1 rounding.
</commit_message>
<xml_diff>
--- a/downloads/DRAC_Input_and_Output_Template.xlsx
+++ b/downloads/DRAC_Input_and_Output_Template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="549">
   <si>
     <t>TI:1</t>
   </si>
@@ -969,6 +969,742 @@
   </si>
   <si>
     <t>Th Alpha grain size absorption factor</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Please cite all uses of DRAC, including the version number, as Durcan, J.A., King, G.E., and Duller, G.A.T., 2015. DRAC: Dose rate and age calculator for trapped charge dating. Quaternary Geochronology, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>XX, XX-XX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Corresponding authors: Julie Durcan (julie.durcan@ouce.ox.ac.uk) and Georgina King (georgina.king@unil.ch).</t>
+    </r>
+  </si>
+  <si>
+    <t>DRAC-example</t>
+  </si>
+  <si>
+    <t>Quartz</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>AdamiecAitken1998</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Brennanetal1991</t>
+  </si>
+  <si>
+    <t>Guerinetal2012-Q</t>
+  </si>
+  <si>
+    <t>Bell1979</t>
+  </si>
+  <si>
+    <t>Feldspar</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Bell1980</t>
+  </si>
+  <si>
+    <t>Mejdahl1979</t>
+  </si>
+  <si>
+    <t>Polymineral</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <r>
+      <t>To calculate dose rates using DRAC, the data table below (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>excluding headers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) can be copied and pasted into the calculator box on the DRAC website (www.aber.ac.uk/alrl/DRAC). Once 'calculate' has been clicked, DRAC will generate an output file, which can be saved by the user.</t>
+    </r>
+  </si>
+  <si>
+    <t>User external alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>User external betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>User external gamma doserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>User internal doserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Scale gammadoserate at shallow depths?</t>
+  </si>
+  <si>
+    <t>Grain size min (microns)</t>
+  </si>
+  <si>
+    <t>Grain size max (microns)</t>
+  </si>
+  <si>
+    <t>alpha-Grain size attenuation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beta-Grain size attenuation </t>
+  </si>
+  <si>
+    <t>Etch depth min (microns)</t>
+  </si>
+  <si>
+    <t>Etch depth max (microns)</t>
+  </si>
+  <si>
+    <t>beta-Etch depth attenuation factor</t>
+  </si>
+  <si>
+    <t>errOverburden density (g cm-3)</t>
+  </si>
+  <si>
+    <t>User cosmicdoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errUser cosmicdoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errDe (Gy)</t>
+  </si>
+  <si>
+    <t>errDepth (m)</t>
+  </si>
+  <si>
+    <t>errWater content %</t>
+  </si>
+  <si>
+    <t>erra-value</t>
+  </si>
+  <si>
+    <t>errUser internal doserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errUser external gammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errUser external betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errUser external alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errRb (ppm)</t>
+  </si>
+  <si>
+    <t>errInternal K (%)</t>
+  </si>
+  <si>
+    <t>errInternal Th (ppm)</t>
+  </si>
+  <si>
+    <t>errInternal U (ppm)</t>
+  </si>
+  <si>
+    <t>errExternal Rb (ppm)</t>
+  </si>
+  <si>
+    <t>errExternal K (%)</t>
+  </si>
+  <si>
+    <t>errExternal Th (ppm)</t>
+  </si>
+  <si>
+    <t>errExternal U (ppm)</t>
+  </si>
+  <si>
+    <t>Attenuated external alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errAttenuated external alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Attenuated external betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errAttenuated external betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Attenuated external gammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errAttenuated external gammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Attenuated internal alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errAttenuated internal alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Attenuated internal betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errAttenuated internal betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errCosmic dose rate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Total external doserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errTotal external doserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Total internal doserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errTotal internal doserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errEnvironmental dose rate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errAge (ka)</t>
+  </si>
+  <si>
+    <t>External U alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External errU alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External U betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External errU betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External U gammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External errU gammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External Th alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External errTh alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External Th betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External errTh betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External Th gammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External errTh gammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External K betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External errK betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External K gammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External errK gammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External Rb betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External errRb betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal U alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal errU alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal U betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal errU betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal Th alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal errTh alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal Th betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal errTh betadoserate (Gy.ka-1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal errK betadoserate (Gy.ka-1) </t>
+  </si>
+  <si>
+    <t>Internal K betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal Rb betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal errRb betadoserate (Gy.ka-1) </t>
+  </si>
+  <si>
+    <t>U gammadoserate scaling factor</t>
+  </si>
+  <si>
+    <t>Th gammadoserate scaling factor</t>
+  </si>
+  <si>
+    <t>K gammadoserate scaling factor</t>
+  </si>
+  <si>
+    <t>Average gammadoserate scaling factor</t>
+  </si>
+  <si>
+    <t>Depth scaled U gammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depth scaled errU gammadoserate (Gy.ka-1) </t>
+  </si>
+  <si>
+    <t>Depth scaled Th gammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depth scaled errTh gammadoserate (Gy.ka-1) </t>
+  </si>
+  <si>
+    <t>Depth scaled K gammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depth scaled errK gammadoserate (Gy.ka-1) </t>
+  </si>
+  <si>
+    <t>Depth scaled user external gammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Depth scaled erruser external gammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External infinite matrix alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External infinite matrix erralphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External infinite matrix betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External infinite matrix errbetadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External infinite matrix gammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External infinite matrix errgammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal infinite matrix alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal infinite matrix erralphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal infinite matrix betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal infinite matrix errbetadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">errU Alpha grain size attenuation factor </t>
+  </si>
+  <si>
+    <t>errTh Alpha grain size attenuation factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">errU Alpha grain size absorption factor </t>
+  </si>
+  <si>
+    <t>errTh Alpha grain size absorption factor</t>
+  </si>
+  <si>
+    <t>Grain size corrected external U alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected external errU alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected external Th alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected external errTh alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected user external alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected user external erralphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected internal U alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected internal errU alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected internal Th alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected internal errTh alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>U-errBeta grain size attenuation factor</t>
+  </si>
+  <si>
+    <t>Th-errBeta grain size attenuation factor</t>
+  </si>
+  <si>
+    <t>K-errBeta grain size attenuation factor</t>
+  </si>
+  <si>
+    <t>Rb-errBeta grain size attenuation factor</t>
+  </si>
+  <si>
+    <t>errCompiled beta grain size attenuation factor</t>
+  </si>
+  <si>
+    <t>U-errBeta grain size absorption factor</t>
+  </si>
+  <si>
+    <t>Th-errBeta grain size absorption factor</t>
+  </si>
+  <si>
+    <t>K-errBeta grain size absorption factor</t>
+  </si>
+  <si>
+    <t>Rb-errBeta grain size absorption factor</t>
+  </si>
+  <si>
+    <t>Grain size corrected external U betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected external errU betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected external Th betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected external errTh betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected external K betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected external errK betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected external Rb betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected external errRb betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected user external betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected user external errbetadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected internal U betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected internal errU betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected internal Th betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected internal errTh betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected internal K betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected internal errK betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected internal Rb betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Grain size corrected internal errRb betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>U-errAlpha Etch attenuation factor</t>
+  </si>
+  <si>
+    <t>Th-errAlpha etch attenuation factor</t>
+  </si>
+  <si>
+    <t>errCompiled alpha etch attenuation factor</t>
+  </si>
+  <si>
+    <t>U-errAlpha Etch absorption factor</t>
+  </si>
+  <si>
+    <t>Th-errAlpha etch absorption factor</t>
+  </si>
+  <si>
+    <t>Etch corrected external U alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected external errU alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected external Th alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected external errTh alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected user external alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected user external erralphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected internal U alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected internal errU alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected internal Th alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected internal errTh alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>U-errBeta etch attenuation factor</t>
+  </si>
+  <si>
+    <t>Th-errBeta etch attenuation factor</t>
+  </si>
+  <si>
+    <t>K-errBeta etch attenuation factor</t>
+  </si>
+  <si>
+    <t>errCompiled beta etch attenuation factor</t>
+  </si>
+  <si>
+    <t>U-errBeta etch absorption factor</t>
+  </si>
+  <si>
+    <t>Th-errBeta etch absorption factor</t>
+  </si>
+  <si>
+    <t>K-errBeta etch absorption factor</t>
+  </si>
+  <si>
+    <t>Etch corrected external U betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected external errU betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected external Th betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected external errTh betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected external K betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected external errK betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected user external betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected user external errbetadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected internal U betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected internal errU betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected internal Th betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected internal errTh betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected internal K betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Etch corrected internal errK betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>a-value corrected external U alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>a-value corrected external errU alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>a-value corrected external Th alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>a-value corrected external errTh alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>a-value corrected user external alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>a-value corrected user external erralphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>a-value corrected internal U alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>a-value corrected internal errU alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>a-value corrected internal Th alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>a-value corrected internal errTh alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External Dry alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External Dry erralphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External Dry betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External Dry errbetadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External Dry gammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External Dry errgammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Water corrected alphadoserate</t>
+  </si>
+  <si>
+    <t>Water corrected erralphadoserate</t>
+  </si>
+  <si>
+    <t>Water corrected betadoserate</t>
+  </si>
+  <si>
+    <t>Water corrected errbetadoserate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water corrected gammadoserate (Gy.ka-1) </t>
+  </si>
+  <si>
+    <t>Water corrected errgammadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal Dry alphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal Dry erralphadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal Dry betadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal Dry errbetadoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>D0 (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errD0 (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Cosmicdoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errCosmicdoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External doserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>External errdoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal doserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>Internal errdoserate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errEnvironmental Dose Rate (Gy.ka-1)</t>
+  </si>
+  <si>
+    <t>errCombined alpha grain size attenuation factor</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
   <si>
     <r>
@@ -999,759 +1735,12 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>XXXX</t>
+      <t>www.aber.ac.uk/alrl/drac</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Please cite all uses of DRAC, including the version number, as Durcan, J.A., King, G.E., and Duller, G.A.T., 2015. DRAC: Dose rate and age calculator for trapped charge dating. Quaternary Geochronology, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>XX, XX-XX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Corresponding authors: Julie Durcan (julie.durcan@ouce.ox.ac.uk) and Georgina King (georgina.king@unil.ch).</t>
-    </r>
-  </si>
-  <si>
-    <t>DRAC-example</t>
-  </si>
-  <si>
-    <t>Quartz</t>
-  </si>
-  <si>
-    <t>Q</t>
-  </si>
-  <si>
-    <t>AdamiecAitken1998</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Brennanetal1991</t>
-  </si>
-  <si>
-    <t>Guerinetal2012-Q</t>
-  </si>
-  <si>
-    <t>Bell1979</t>
-  </si>
-  <si>
-    <t>Feldspar</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Bell1980</t>
-  </si>
-  <si>
-    <t>Mejdahl1979</t>
-  </si>
-  <si>
-    <t>Polymineral</t>
-  </si>
-  <si>
-    <t>PM</t>
-  </si>
-  <si>
-    <r>
-      <t>To calculate dose rates using DRAC, the data table below (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>excluding headers</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) can be copied and pasted into the calculator box on the DRAC website (www.aber.ac.uk/alrl/DRAC). Once 'calculate' has been clicked, DRAC will generate an output file, which can be saved by the user.</t>
-    </r>
-  </si>
-  <si>
-    <t>User external alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>User external betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>User external gamma doserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>User internal doserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Scale gammadoserate at shallow depths?</t>
-  </si>
-  <si>
-    <t>Grain size min (microns)</t>
-  </si>
-  <si>
-    <t>Grain size max (microns)</t>
-  </si>
-  <si>
-    <t>alpha-Grain size attenuation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">beta-Grain size attenuation </t>
-  </si>
-  <si>
-    <t>Etch depth min (microns)</t>
-  </si>
-  <si>
-    <t>Etch depth max (microns)</t>
-  </si>
-  <si>
-    <t>beta-Etch depth attenuation factor</t>
-  </si>
-  <si>
-    <t>errOverburden density (g cm-3)</t>
-  </si>
-  <si>
-    <t>User cosmicdoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errUser cosmicdoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errDe (Gy)</t>
-  </si>
-  <si>
-    <t>errDepth (m)</t>
-  </si>
-  <si>
-    <t>errWater content %</t>
-  </si>
-  <si>
-    <t>erra-value</t>
-  </si>
-  <si>
-    <t>errUser internal doserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errUser external gammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errUser external betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errUser external alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errRb (ppm)</t>
-  </si>
-  <si>
-    <t>errInternal K (%)</t>
-  </si>
-  <si>
-    <t>errInternal Th (ppm)</t>
-  </si>
-  <si>
-    <t>errInternal U (ppm)</t>
-  </si>
-  <si>
-    <t>errExternal Rb (ppm)</t>
-  </si>
-  <si>
-    <t>errExternal K (%)</t>
-  </si>
-  <si>
-    <t>errExternal Th (ppm)</t>
-  </si>
-  <si>
-    <t>errExternal U (ppm)</t>
-  </si>
-  <si>
-    <t>Attenuated external alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errAttenuated external alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Attenuated external betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errAttenuated external betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Attenuated external gammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errAttenuated external gammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Attenuated internal alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errAttenuated internal alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Attenuated internal betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errAttenuated internal betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errCosmic dose rate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Total external doserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errTotal external doserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Total internal doserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errTotal internal doserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errEnvironmental dose rate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errAge (ka)</t>
-  </si>
-  <si>
-    <t>External U alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External errU alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External U betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External errU betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External U gammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External errU gammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External Th alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External errTh alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External Th betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External errTh betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External Th gammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External errTh gammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External K betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External errK betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External K gammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External errK gammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External Rb betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External errRb betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal U alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal errU alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal U betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal errU betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal Th alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal errTh alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal Th betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Internal errTh betadoserate (Gy.ka-1) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Internal errK betadoserate (Gy.ka-1) </t>
-  </si>
-  <si>
-    <t>Internal K betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal Rb betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Internal errRb betadoserate (Gy.ka-1) </t>
-  </si>
-  <si>
-    <t>U gammadoserate scaling factor</t>
-  </si>
-  <si>
-    <t>Th gammadoserate scaling factor</t>
-  </si>
-  <si>
-    <t>K gammadoserate scaling factor</t>
-  </si>
-  <si>
-    <t>Average gammadoserate scaling factor</t>
-  </si>
-  <si>
-    <t>Depth scaled U gammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth scaled errU gammadoserate (Gy.ka-1) </t>
-  </si>
-  <si>
-    <t>Depth scaled Th gammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth scaled errTh gammadoserate (Gy.ka-1) </t>
-  </si>
-  <si>
-    <t>Depth scaled K gammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Depth scaled errK gammadoserate (Gy.ka-1) </t>
-  </si>
-  <si>
-    <t>Depth scaled user external gammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Depth scaled erruser external gammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External infinite matrix alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External infinite matrix erralphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External infinite matrix betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External infinite matrix errbetadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External infinite matrix gammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External infinite matrix errgammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal infinite matrix alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal infinite matrix erralphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal infinite matrix betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal infinite matrix errbetadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">errU Alpha grain size attenuation factor </t>
-  </si>
-  <si>
-    <t>errTh Alpha grain size attenuation factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">errU Alpha grain size absorption factor </t>
-  </si>
-  <si>
-    <t>errTh Alpha grain size absorption factor</t>
-  </si>
-  <si>
-    <t>Grain size corrected external U alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected external errU alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected external Th alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected external errTh alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected user external alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected user external erralphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected internal U alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected internal errU alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected internal Th alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected internal errTh alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>U-errBeta grain size attenuation factor</t>
-  </si>
-  <si>
-    <t>Th-errBeta grain size attenuation factor</t>
-  </si>
-  <si>
-    <t>K-errBeta grain size attenuation factor</t>
-  </si>
-  <si>
-    <t>Rb-errBeta grain size attenuation factor</t>
-  </si>
-  <si>
-    <t>errCompiled beta grain size attenuation factor</t>
-  </si>
-  <si>
-    <t>U-errBeta grain size absorption factor</t>
-  </si>
-  <si>
-    <t>Th-errBeta grain size absorption factor</t>
-  </si>
-  <si>
-    <t>K-errBeta grain size absorption factor</t>
-  </si>
-  <si>
-    <t>Rb-errBeta grain size absorption factor</t>
-  </si>
-  <si>
-    <t>Grain size corrected external U betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected external errU betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected external Th betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected external errTh betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected external K betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected external errK betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected external Rb betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected external errRb betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected user external betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected user external errbetadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected internal U betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected internal errU betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected internal Th betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected internal errTh betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected internal K betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected internal errK betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected internal Rb betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Grain size corrected internal errRb betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>U-errAlpha Etch attenuation factor</t>
-  </si>
-  <si>
-    <t>Th-errAlpha etch attenuation factor</t>
-  </si>
-  <si>
-    <t>errCompiled alpha etch attenuation factor</t>
-  </si>
-  <si>
-    <t>U-errAlpha Etch absorption factor</t>
-  </si>
-  <si>
-    <t>Th-errAlpha etch absorption factor</t>
-  </si>
-  <si>
-    <t>Etch corrected external U alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected external errU alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected external Th alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected external errTh alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected user external alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected user external erralphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected internal U alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected internal errU alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected internal Th alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected internal errTh alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>U-errBeta etch attenuation factor</t>
-  </si>
-  <si>
-    <t>Th-errBeta etch attenuation factor</t>
-  </si>
-  <si>
-    <t>K-errBeta etch attenuation factor</t>
-  </si>
-  <si>
-    <t>errCompiled beta etch attenuation factor</t>
-  </si>
-  <si>
-    <t>U-errBeta etch absorption factor</t>
-  </si>
-  <si>
-    <t>Th-errBeta etch absorption factor</t>
-  </si>
-  <si>
-    <t>K-errBeta etch absorption factor</t>
-  </si>
-  <si>
-    <t>Etch corrected external U betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected external errU betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected external Th betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected external errTh betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected external K betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected external errK betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected user external betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected user external errbetadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected internal U betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected internal errU betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected internal Th betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected internal errTh betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected internal K betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Etch corrected internal errK betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>a-value corrected external U alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>a-value corrected external errU alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>a-value corrected external Th alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>a-value corrected external errTh alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>a-value corrected user external alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>a-value corrected user external erralphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>a-value corrected internal U alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>a-value corrected internal errU alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>a-value corrected internal Th alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>a-value corrected internal errTh alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External Dry alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External Dry erralphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External Dry betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External Dry errbetadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External Dry gammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External Dry errgammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Water corrected alphadoserate</t>
-  </si>
-  <si>
-    <t>Water corrected erralphadoserate</t>
-  </si>
-  <si>
-    <t>Water corrected betadoserate</t>
-  </si>
-  <si>
-    <t>Water corrected errbetadoserate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water corrected gammadoserate (Gy.ka-1) </t>
-  </si>
-  <si>
-    <t>Water corrected errgammadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal Dry alphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal Dry erralphadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal Dry betadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal Dry errbetadoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>D0 (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errD0 (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Cosmicdoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errCosmicdoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External doserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>External errdoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal doserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>Internal errdoserate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errEnvironmental Dose Rate (Gy.ka-1)</t>
-  </si>
-  <si>
-    <t>errCombined alpha grain size attenuation factor</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
 </sst>
 </file>
@@ -1762,7 +1751,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1820,6 +1809,13 @@
       <i/>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2195,8 +2191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
-      <selection activeCell="BA14" sqref="A12:BA14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2268,17 +2264,17 @@
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>318</v>
+        <v>548</v>
       </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.25">
@@ -2459,25 +2455,25 @@
         <v>8</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>20</v>
@@ -2486,100 +2482,100 @@
         <v>22</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>25</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="R11" s="6" t="s">
         <v>28</v>
       </c>
       <c r="S11" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="T11" s="6" t="s">
         <v>31</v>
       </c>
       <c r="U11" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="V11" s="6" t="s">
         <v>34</v>
       </c>
       <c r="W11" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="X11" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="Y11" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="X11" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="Y11" s="6" t="s">
+      <c r="Z11" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="AA11" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="Z11" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="AA11" s="6" t="s">
+      <c r="AB11" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="AC11" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="AB11" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="AC11" s="6" t="s">
+      <c r="AD11" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="AE11" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="AD11" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="AE11" s="6" t="s">
+      <c r="AF11" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="AF11" s="6" t="s">
+      <c r="AG11" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="AG11" s="6" t="s">
+      <c r="AH11" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="AH11" s="6" t="s">
+      <c r="AI11" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="AI11" s="6" t="s">
+      <c r="AJ11" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="AJ11" s="6" t="s">
+      <c r="AK11" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="AK11" s="6" t="s">
+      <c r="AL11" s="6" t="s">
         <v>345</v>
-      </c>
-      <c r="AL11" s="6" t="s">
-        <v>346</v>
       </c>
       <c r="AM11" s="6" t="s">
         <v>50</v>
       </c>
       <c r="AN11" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AO11" s="6" t="s">
         <v>53</v>
       </c>
       <c r="AP11" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AQ11" s="6" t="s">
         <v>56</v>
       </c>
       <c r="AR11" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AS11" s="6" t="s">
         <v>59</v>
       </c>
       <c r="AT11" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AU11" s="6" t="s">
         <v>62</v>
@@ -2591,30 +2587,30 @@
         <v>66</v>
       </c>
       <c r="AX11" s="6" t="s">
+        <v>347</v>
+      </c>
+      <c r="AY11" s="6" t="s">
         <v>348</v>
-      </c>
-      <c r="AY11" s="6" t="s">
-        <v>349</v>
       </c>
       <c r="AZ11" s="6" t="s">
         <v>70</v>
       </c>
       <c r="BA11" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>320</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="C12" s="18" t="s">
         <v>321</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="D12" s="17" t="s">
         <v>322</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>323</v>
       </c>
       <c r="E12" s="17">
         <v>3.4</v>
@@ -2641,61 +2637,61 @@
         <v>0</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="O12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="Q12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="R12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="S12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="T12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="U12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="V12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="W12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="X12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="Y12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="Z12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AA12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AB12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AC12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AD12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AE12" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AF12" s="17">
         <v>90</v>
@@ -2704,10 +2700,10 @@
         <v>125</v>
       </c>
       <c r="AH12" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="AI12" s="17" t="s">
         <v>325</v>
-      </c>
-      <c r="AI12" s="17" t="s">
-        <v>326</v>
       </c>
       <c r="AJ12" s="17">
         <v>8</v>
@@ -2716,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="AL12" s="17" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AM12" s="17">
         <v>0</v>
@@ -2752,10 +2748,10 @@
         <v>150</v>
       </c>
       <c r="AX12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AY12" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AZ12" s="17">
         <v>20</v>
@@ -2766,16 +2762,16 @@
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>285</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E13" s="17">
         <v>2</v>
@@ -2802,19 +2798,19 @@
         <v>0</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N13" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="O13" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="P13" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="Q13" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="R13" s="17">
         <v>12.5</v>
@@ -2823,40 +2819,40 @@
         <v>0.5</v>
       </c>
       <c r="T13" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="U13" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="V13" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W13" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="X13" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="Y13" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="Z13" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AA13" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AB13" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AC13" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AD13" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AE13" s="17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AF13" s="17">
         <v>180</v>
@@ -2865,10 +2861,10 @@
         <v>212</v>
       </c>
       <c r="AH13" s="17" t="s">
+        <v>329</v>
+      </c>
+      <c r="AI13" s="17" t="s">
         <v>330</v>
-      </c>
-      <c r="AI13" s="17" t="s">
-        <v>331</v>
       </c>
       <c r="AJ13" s="17">
         <v>0</v>
@@ -2877,7 +2873,7 @@
         <v>0</v>
       </c>
       <c r="AL13" s="17" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AM13" s="17">
         <v>0.15</v>
@@ -2913,10 +2909,10 @@
         <v>200</v>
       </c>
       <c r="AX13" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AY13" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AZ13" s="17">
         <v>15</v>
@@ -2927,16 +2923,16 @@
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B14" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>332</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>333</v>
-      </c>
       <c r="D14" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E14" s="17">
         <v>4</v>
@@ -2963,19 +2959,19 @@
         <v>0</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="P14" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="Q14" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="R14" s="17">
         <v>12.5</v>
@@ -2984,19 +2980,19 @@
         <v>0.5</v>
       </c>
       <c r="T14" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="U14" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="V14" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W14" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="X14" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="Y14" s="17">
         <v>2.5</v>
@@ -3005,19 +3001,19 @@
         <v>0.15</v>
       </c>
       <c r="AA14" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AB14" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AC14" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AD14" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AE14" s="17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AF14" s="17">
         <v>4</v>
@@ -3026,10 +3022,10 @@
         <v>11</v>
       </c>
       <c r="AH14" s="17" t="s">
+        <v>329</v>
+      </c>
+      <c r="AI14" s="17" t="s">
         <v>330</v>
-      </c>
-      <c r="AI14" s="17" t="s">
-        <v>331</v>
       </c>
       <c r="AJ14" s="17">
         <v>0</v>
@@ -3038,7 +3034,7 @@
         <v>0</v>
       </c>
       <c r="AL14" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AM14" s="17">
         <v>8.5999999999999993E-2</v>
@@ -3052,26 +3048,26 @@
       <c r="AP14" s="17">
         <v>5</v>
       </c>
-      <c r="AQ14" s="17">
-        <v>0.2</v>
-      </c>
-      <c r="AR14" s="17">
-        <v>0.02</v>
-      </c>
-      <c r="AS14" s="17">
-        <v>1.8</v>
-      </c>
-      <c r="AT14" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="AU14" s="17">
-        <v>46</v>
-      </c>
-      <c r="AV14" s="17">
-        <v>118</v>
-      </c>
-      <c r="AW14" s="17">
-        <v>200</v>
+      <c r="AQ14" s="17" t="s">
+        <v>547</v>
+      </c>
+      <c r="AR14" s="17" t="s">
+        <v>547</v>
+      </c>
+      <c r="AS14" s="17" t="s">
+        <v>547</v>
+      </c>
+      <c r="AT14" s="17" t="s">
+        <v>547</v>
+      </c>
+      <c r="AU14" s="17" t="s">
+        <v>547</v>
+      </c>
+      <c r="AV14" s="17" t="s">
+        <v>547</v>
+      </c>
+      <c r="AW14" s="17" t="s">
+        <v>547</v>
       </c>
       <c r="AX14" s="17">
         <v>0.2</v>
@@ -3095,8 +3091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:JT277"/>
   <sheetViews>
-    <sheetView topLeftCell="JK1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="JM16" sqref="JM16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3389,12 +3385,12 @@
     </row>
     <row r="4" spans="1:280" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>318</v>
+        <v>548</v>
       </c>
     </row>
     <row r="6" spans="1:280" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="8" spans="1:280" x14ac:dyDescent="0.25">
@@ -4259,70 +4255,70 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
+        <v>365</v>
+      </c>
+      <c r="E14" t="s">
         <v>366</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>367</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>368</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>369</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>370</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>371</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>372</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>373</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>374</v>
-      </c>
-      <c r="M14" t="s">
-        <v>375</v>
       </c>
       <c r="N14" t="s">
         <v>288</v>
       </c>
       <c r="O14" t="s">
+        <v>375</v>
+      </c>
+      <c r="P14" t="s">
         <v>376</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>377</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>378</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>379</v>
-      </c>
-      <c r="S14" t="s">
-        <v>380</v>
       </c>
       <c r="T14" t="s">
         <v>310</v>
       </c>
       <c r="U14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="V14" t="s">
         <v>70</v>
       </c>
       <c r="W14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="X14" t="s">
         <v>292</v>
       </c>
       <c r="Y14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AB14" s="12" t="s">
         <v>306</v>
@@ -4340,25 +4336,25 @@
         <v>8</v>
       </c>
       <c r="AG14" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AH14" s="14" t="s">
         <v>11</v>
       </c>
       <c r="AI14" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AJ14" s="14" t="s">
         <v>14</v>
       </c>
       <c r="AK14" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AL14" s="14" t="s">
         <v>17</v>
       </c>
       <c r="AM14" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AN14" s="14" t="s">
         <v>20</v>
@@ -4367,100 +4363,100 @@
         <v>22</v>
       </c>
       <c r="AP14" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="AQ14" s="14" t="s">
         <v>25</v>
       </c>
       <c r="AR14" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AS14" s="14" t="s">
         <v>28</v>
       </c>
       <c r="AT14" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AU14" s="14" t="s">
         <v>31</v>
       </c>
       <c r="AV14" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AW14" s="14" t="s">
         <v>34</v>
       </c>
       <c r="AX14" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="AY14" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="AZ14" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="AY14" s="14" t="s">
-        <v>357</v>
-      </c>
-      <c r="AZ14" s="14" t="s">
+      <c r="BA14" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="BB14" s="14" t="s">
         <v>336</v>
       </c>
-      <c r="BA14" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="BB14" s="14" t="s">
+      <c r="BC14" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="BD14" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="BC14" s="14" t="s">
-        <v>355</v>
-      </c>
-      <c r="BD14" s="14" t="s">
+      <c r="BE14" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="BF14" s="14" t="s">
         <v>338</v>
       </c>
-      <c r="BE14" s="14" t="s">
-        <v>354</v>
-      </c>
-      <c r="BF14" s="14" t="s">
+      <c r="BG14" s="14" t="s">
         <v>339</v>
       </c>
-      <c r="BG14" s="14" t="s">
+      <c r="BH14" s="14" t="s">
         <v>340</v>
       </c>
-      <c r="BH14" s="14" t="s">
+      <c r="BI14" s="14" t="s">
         <v>341</v>
       </c>
-      <c r="BI14" s="14" t="s">
+      <c r="BJ14" s="14" t="s">
         <v>342</v>
       </c>
-      <c r="BJ14" s="14" t="s">
+      <c r="BK14" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="BK14" s="14" t="s">
+      <c r="BL14" s="14" t="s">
         <v>344</v>
       </c>
-      <c r="BL14" s="14" t="s">
+      <c r="BM14" s="14" t="s">
         <v>345</v>
-      </c>
-      <c r="BM14" s="14" t="s">
-        <v>346</v>
       </c>
       <c r="BN14" s="14" t="s">
         <v>50</v>
       </c>
       <c r="BO14" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="BP14" s="14" t="s">
         <v>53</v>
       </c>
       <c r="BQ14" s="14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BR14" s="14" t="s">
         <v>56</v>
       </c>
       <c r="BS14" s="14" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="BT14" s="14" t="s">
         <v>59</v>
       </c>
       <c r="BU14" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="BV14" s="14" t="s">
         <v>62</v>
@@ -4472,569 +4468,569 @@
         <v>66</v>
       </c>
       <c r="BY14" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="BZ14" s="14" t="s">
         <v>348</v>
-      </c>
-      <c r="BZ14" s="14" t="s">
-        <v>349</v>
       </c>
       <c r="CA14" s="14" t="s">
         <v>70</v>
       </c>
       <c r="CB14" s="14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="CC14" s="11"/>
       <c r="CE14" t="s">
+        <v>382</v>
+      </c>
+      <c r="CF14" t="s">
         <v>383</v>
       </c>
-      <c r="CF14" t="s">
+      <c r="CG14" t="s">
         <v>384</v>
       </c>
-      <c r="CG14" t="s">
+      <c r="CH14" t="s">
         <v>385</v>
       </c>
-      <c r="CH14" t="s">
+      <c r="CI14" t="s">
         <v>386</v>
       </c>
-      <c r="CI14" t="s">
+      <c r="CJ14" t="s">
         <v>387</v>
       </c>
-      <c r="CJ14" t="s">
+      <c r="CK14" t="s">
         <v>388</v>
       </c>
-      <c r="CK14" t="s">
+      <c r="CL14" t="s">
         <v>389</v>
       </c>
-      <c r="CL14" t="s">
+      <c r="CM14" t="s">
         <v>390</v>
       </c>
-      <c r="CM14" t="s">
+      <c r="CN14" t="s">
         <v>391</v>
       </c>
-      <c r="CN14" t="s">
+      <c r="CO14" t="s">
         <v>392</v>
       </c>
-      <c r="CO14" t="s">
+      <c r="CP14" t="s">
         <v>393</v>
       </c>
-      <c r="CP14" t="s">
+      <c r="CQ14" t="s">
         <v>394</v>
       </c>
-      <c r="CQ14" t="s">
+      <c r="CR14" t="s">
         <v>395</v>
       </c>
-      <c r="CR14" t="s">
+      <c r="CS14" t="s">
         <v>396</v>
       </c>
-      <c r="CS14" t="s">
+      <c r="CT14" t="s">
         <v>397</v>
       </c>
-      <c r="CT14" t="s">
+      <c r="CU14" t="s">
         <v>398</v>
       </c>
-      <c r="CU14" t="s">
+      <c r="CV14" t="s">
         <v>399</v>
       </c>
-      <c r="CV14" t="s">
+      <c r="CW14" t="s">
         <v>400</v>
       </c>
-      <c r="CW14" t="s">
+      <c r="CX14" t="s">
         <v>401</v>
       </c>
-      <c r="CX14" t="s">
+      <c r="CY14" t="s">
         <v>402</v>
       </c>
-      <c r="CY14" t="s">
+      <c r="CZ14" t="s">
         <v>403</v>
       </c>
-      <c r="CZ14" t="s">
+      <c r="DA14" t="s">
         <v>404</v>
       </c>
-      <c r="DA14" t="s">
+      <c r="DB14" t="s">
         <v>405</v>
       </c>
-      <c r="DB14" t="s">
+      <c r="DC14" t="s">
         <v>406</v>
       </c>
-      <c r="DC14" t="s">
+      <c r="DD14" t="s">
         <v>407</v>
       </c>
-      <c r="DD14" t="s">
+      <c r="DE14" t="s">
+        <v>409</v>
+      </c>
+      <c r="DF14" s="15" t="s">
         <v>408</v>
       </c>
-      <c r="DE14" t="s">
+      <c r="DG14" t="s">
         <v>410</v>
       </c>
-      <c r="DF14" s="15" t="s">
-        <v>409</v>
-      </c>
-      <c r="DG14" t="s">
+      <c r="DH14" t="s">
         <v>411</v>
       </c>
-      <c r="DH14" t="s">
+      <c r="DI14" t="s">
         <v>412</v>
       </c>
-      <c r="DI14" t="s">
+      <c r="DJ14" t="s">
         <v>413</v>
       </c>
-      <c r="DJ14" t="s">
+      <c r="DK14" t="s">
         <v>414</v>
       </c>
-      <c r="DK14" t="s">
+      <c r="DL14" t="s">
         <v>415</v>
       </c>
-      <c r="DL14" t="s">
+      <c r="DM14" t="s">
         <v>416</v>
       </c>
-      <c r="DM14" t="s">
+      <c r="DN14" t="s">
         <v>417</v>
       </c>
-      <c r="DN14" t="s">
+      <c r="DO14" t="s">
         <v>418</v>
       </c>
-      <c r="DO14" t="s">
+      <c r="DP14" t="s">
         <v>419</v>
       </c>
-      <c r="DP14" t="s">
+      <c r="DQ14" t="s">
         <v>420</v>
       </c>
-      <c r="DQ14" t="s">
+      <c r="DR14" t="s">
         <v>421</v>
       </c>
-      <c r="DR14" t="s">
+      <c r="DS14" t="s">
         <v>422</v>
       </c>
-      <c r="DS14" t="s">
+      <c r="DT14" t="s">
         <v>423</v>
       </c>
-      <c r="DT14" t="s">
+      <c r="DU14" t="s">
         <v>424</v>
       </c>
-      <c r="DU14" t="s">
+      <c r="DV14" t="s">
         <v>425</v>
       </c>
-      <c r="DV14" t="s">
+      <c r="DW14" t="s">
         <v>426</v>
       </c>
-      <c r="DW14" t="s">
+      <c r="DX14" t="s">
         <v>427</v>
       </c>
-      <c r="DX14" t="s">
+      <c r="DY14" t="s">
         <v>428</v>
       </c>
-      <c r="DY14" t="s">
+      <c r="DZ14" t="s">
         <v>429</v>
       </c>
-      <c r="DZ14" t="s">
+      <c r="EA14" t="s">
         <v>430</v>
       </c>
-      <c r="EA14" t="s">
+      <c r="EB14" t="s">
         <v>431</v>
       </c>
-      <c r="EB14" t="s">
+      <c r="EC14" t="s">
         <v>432</v>
       </c>
-      <c r="EC14" t="s">
+      <c r="ED14" t="s">
         <v>433</v>
-      </c>
-      <c r="ED14" t="s">
-        <v>434</v>
       </c>
       <c r="EE14" t="s">
         <v>313</v>
       </c>
       <c r="EF14" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="EG14" t="s">
         <v>314</v>
       </c>
       <c r="EH14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="EI14" t="s">
         <v>315</v>
       </c>
       <c r="EJ14" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="EK14" t="s">
         <v>316</v>
       </c>
       <c r="EL14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="EM14" t="s">
         <v>317</v>
       </c>
       <c r="EN14" t="s">
+        <v>437</v>
+      </c>
+      <c r="EO14" t="s">
         <v>438</v>
       </c>
-      <c r="EO14" t="s">
+      <c r="EP14" t="s">
         <v>439</v>
       </c>
-      <c r="EP14" t="s">
+      <c r="EQ14" t="s">
         <v>440</v>
       </c>
-      <c r="EQ14" t="s">
+      <c r="ER14" t="s">
         <v>441</v>
       </c>
-      <c r="ER14" t="s">
+      <c r="ES14" t="s">
         <v>442</v>
       </c>
-      <c r="ES14" t="s">
+      <c r="ET14" t="s">
         <v>443</v>
       </c>
-      <c r="ET14" t="s">
+      <c r="EU14" t="s">
         <v>444</v>
       </c>
-      <c r="EU14" t="s">
+      <c r="EV14" t="s">
         <v>445</v>
       </c>
-      <c r="EV14" t="s">
+      <c r="EW14" t="s">
         <v>446</v>
       </c>
-      <c r="EW14" t="s">
+      <c r="EX14" t="s">
         <v>447</v>
-      </c>
-      <c r="EX14" t="s">
-        <v>448</v>
       </c>
       <c r="EY14" t="s">
         <v>263</v>
       </c>
       <c r="EZ14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="FA14" t="s">
         <v>264</v>
       </c>
       <c r="FB14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="FC14" t="s">
         <v>265</v>
       </c>
       <c r="FD14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="FE14" t="s">
         <v>266</v>
       </c>
       <c r="FF14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="FG14" t="s">
         <v>267</v>
       </c>
       <c r="FH14" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="FI14" t="s">
         <v>268</v>
       </c>
       <c r="FJ14" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="FK14" t="s">
         <v>269</v>
       </c>
       <c r="FL14" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="FM14" t="s">
         <v>270</v>
       </c>
       <c r="FN14" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="FO14" t="s">
         <v>271</v>
       </c>
       <c r="FP14" t="s">
+        <v>456</v>
+      </c>
+      <c r="FQ14" t="s">
         <v>457</v>
       </c>
-      <c r="FQ14" t="s">
+      <c r="FR14" t="s">
         <v>458</v>
       </c>
-      <c r="FR14" t="s">
+      <c r="FS14" t="s">
         <v>459</v>
       </c>
-      <c r="FS14" t="s">
+      <c r="FT14" t="s">
         <v>460</v>
       </c>
-      <c r="FT14" t="s">
+      <c r="FU14" t="s">
         <v>461</v>
       </c>
-      <c r="FU14" t="s">
+      <c r="FV14" t="s">
         <v>462</v>
       </c>
-      <c r="FV14" t="s">
+      <c r="FW14" t="s">
         <v>463</v>
       </c>
-      <c r="FW14" t="s">
+      <c r="FX14" t="s">
         <v>464</v>
       </c>
-      <c r="FX14" t="s">
+      <c r="FY14" t="s">
         <v>465</v>
       </c>
-      <c r="FY14" t="s">
+      <c r="FZ14" t="s">
         <v>466</v>
       </c>
-      <c r="FZ14" t="s">
+      <c r="GA14" t="s">
         <v>467</v>
       </c>
-      <c r="GA14" t="s">
+      <c r="GB14" t="s">
         <v>468</v>
       </c>
-      <c r="GB14" t="s">
+      <c r="GC14" t="s">
         <v>469</v>
       </c>
-      <c r="GC14" t="s">
+      <c r="GD14" t="s">
         <v>470</v>
       </c>
-      <c r="GD14" t="s">
+      <c r="GE14" t="s">
         <v>471</v>
       </c>
-      <c r="GE14" t="s">
+      <c r="GF14" t="s">
         <v>472</v>
       </c>
-      <c r="GF14" t="s">
+      <c r="GG14" t="s">
         <v>473</v>
       </c>
-      <c r="GG14" t="s">
+      <c r="GH14" t="s">
         <v>474</v>
-      </c>
-      <c r="GH14" t="s">
-        <v>475</v>
       </c>
       <c r="GI14" t="s">
         <v>272</v>
       </c>
       <c r="GJ14" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="GK14" t="s">
         <v>273</v>
       </c>
       <c r="GL14" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="GM14" t="s">
         <v>274</v>
       </c>
       <c r="GN14" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="GO14" t="s">
         <v>275</v>
       </c>
       <c r="GP14" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="GQ14" t="s">
         <v>276</v>
       </c>
       <c r="GR14" t="s">
+        <v>479</v>
+      </c>
+      <c r="GS14" t="s">
         <v>480</v>
       </c>
-      <c r="GS14" t="s">
+      <c r="GT14" t="s">
         <v>481</v>
       </c>
-      <c r="GT14" t="s">
+      <c r="GU14" t="s">
         <v>482</v>
       </c>
-      <c r="GU14" t="s">
+      <c r="GV14" t="s">
         <v>483</v>
       </c>
-      <c r="GV14" t="s">
+      <c r="GW14" t="s">
         <v>484</v>
       </c>
-      <c r="GW14" t="s">
+      <c r="GX14" t="s">
         <v>485</v>
       </c>
-      <c r="GX14" t="s">
+      <c r="GY14" t="s">
         <v>486</v>
       </c>
-      <c r="GY14" t="s">
+      <c r="GZ14" t="s">
         <v>487</v>
       </c>
-      <c r="GZ14" t="s">
+      <c r="HA14" t="s">
         <v>488</v>
       </c>
-      <c r="HA14" t="s">
+      <c r="HB14" t="s">
         <v>489</v>
-      </c>
-      <c r="HB14" t="s">
-        <v>490</v>
       </c>
       <c r="HC14" t="s">
         <v>277</v>
       </c>
       <c r="HD14" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="HE14" t="s">
         <v>278</v>
       </c>
       <c r="HF14" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="HG14" t="s">
         <v>279</v>
       </c>
       <c r="HH14" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="HI14" t="s">
         <v>280</v>
       </c>
       <c r="HJ14" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="HK14" t="s">
         <v>281</v>
       </c>
       <c r="HL14" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="HM14" t="s">
         <v>282</v>
       </c>
       <c r="HN14" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="HO14" t="s">
         <v>283</v>
       </c>
       <c r="HP14" t="s">
+        <v>496</v>
+      </c>
+      <c r="HQ14" t="s">
         <v>497</v>
       </c>
-      <c r="HQ14" t="s">
+      <c r="HR14" t="s">
         <v>498</v>
       </c>
-      <c r="HR14" t="s">
+      <c r="HS14" t="s">
         <v>499</v>
       </c>
-      <c r="HS14" t="s">
+      <c r="HT14" t="s">
         <v>500</v>
       </c>
-      <c r="HT14" t="s">
+      <c r="HU14" t="s">
         <v>501</v>
       </c>
-      <c r="HU14" t="s">
+      <c r="HV14" t="s">
         <v>502</v>
       </c>
-      <c r="HV14" t="s">
+      <c r="HW14" t="s">
         <v>503</v>
       </c>
-      <c r="HW14" t="s">
+      <c r="HX14" t="s">
         <v>504</v>
       </c>
-      <c r="HX14" t="s">
+      <c r="HY14" t="s">
         <v>505</v>
       </c>
-      <c r="HY14" t="s">
+      <c r="HZ14" t="s">
         <v>506</v>
       </c>
-      <c r="HZ14" t="s">
+      <c r="IA14" t="s">
         <v>507</v>
       </c>
-      <c r="IA14" t="s">
+      <c r="IB14" t="s">
         <v>508</v>
       </c>
-      <c r="IB14" t="s">
+      <c r="IC14" t="s">
         <v>509</v>
       </c>
-      <c r="IC14" t="s">
+      <c r="ID14" t="s">
         <v>510</v>
       </c>
-      <c r="ID14" t="s">
+      <c r="IE14" t="s">
         <v>511</v>
       </c>
-      <c r="IE14" t="s">
+      <c r="IF14" t="s">
         <v>512</v>
       </c>
-      <c r="IF14" t="s">
+      <c r="IG14" t="s">
         <v>513</v>
       </c>
-      <c r="IG14" t="s">
+      <c r="IH14" t="s">
         <v>514</v>
       </c>
-      <c r="IH14" t="s">
+      <c r="II14" t="s">
         <v>515</v>
       </c>
-      <c r="II14" t="s">
+      <c r="IJ14" t="s">
         <v>516</v>
       </c>
-      <c r="IJ14" t="s">
+      <c r="IK14" t="s">
         <v>517</v>
       </c>
-      <c r="IK14" t="s">
+      <c r="IL14" t="s">
         <v>518</v>
       </c>
-      <c r="IL14" t="s">
+      <c r="IM14" t="s">
         <v>519</v>
       </c>
-      <c r="IM14" t="s">
+      <c r="IN14" t="s">
         <v>520</v>
       </c>
-      <c r="IN14" t="s">
+      <c r="IO14" t="s">
         <v>521</v>
       </c>
-      <c r="IO14" t="s">
+      <c r="IP14" t="s">
         <v>522</v>
       </c>
-      <c r="IP14" t="s">
+      <c r="IQ14" t="s">
         <v>523</v>
       </c>
-      <c r="IQ14" t="s">
+      <c r="IR14" t="s">
         <v>524</v>
       </c>
-      <c r="IR14" t="s">
+      <c r="IS14" t="s">
         <v>525</v>
       </c>
-      <c r="IS14" t="s">
+      <c r="IT14" t="s">
         <v>526</v>
       </c>
-      <c r="IT14" t="s">
+      <c r="IU14" t="s">
         <v>527</v>
       </c>
-      <c r="IU14" t="s">
+      <c r="IV14" t="s">
         <v>528</v>
       </c>
-      <c r="IV14" t="s">
+      <c r="IW14" t="s">
         <v>529</v>
       </c>
-      <c r="IW14" t="s">
+      <c r="IX14" t="s">
         <v>530</v>
       </c>
-      <c r="IX14" t="s">
+      <c r="IY14" t="s">
         <v>531</v>
       </c>
-      <c r="IY14" t="s">
+      <c r="IZ14" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="IZ14" s="4" t="s">
+      <c r="JA14" t="s">
         <v>533</v>
       </c>
-      <c r="JA14" t="s">
+      <c r="JB14" t="s">
         <v>534</v>
       </c>
-      <c r="JB14" t="s">
+      <c r="JC14" t="s">
         <v>535</v>
       </c>
-      <c r="JC14" t="s">
+      <c r="JD14" t="s">
         <v>536</v>
       </c>
-      <c r="JD14" t="s">
+      <c r="JE14" t="s">
         <v>537</v>
       </c>
-      <c r="JE14" t="s">
+      <c r="JF14" t="s">
         <v>538</v>
-      </c>
-      <c r="JF14" t="s">
-        <v>539</v>
       </c>
       <c r="JG14" t="s">
         <v>284</v>
@@ -5049,34 +5045,34 @@
         <v>287</v>
       </c>
       <c r="JK14" t="s">
+        <v>539</v>
+      </c>
+      <c r="JL14" t="s">
         <v>540</v>
       </c>
-      <c r="JL14" t="s">
+      <c r="JM14" t="s">
         <v>541</v>
       </c>
-      <c r="JM14" t="s">
+      <c r="JN14" t="s">
         <v>542</v>
       </c>
-      <c r="JN14" t="s">
+      <c r="JO14" t="s">
         <v>543</v>
       </c>
-      <c r="JO14" t="s">
+      <c r="JP14" t="s">
         <v>544</v>
-      </c>
-      <c r="JP14" t="s">
-        <v>545</v>
       </c>
       <c r="JQ14" t="s">
         <v>289</v>
       </c>
       <c r="JR14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="JS14" t="s">
         <v>292</v>
       </c>
       <c r="JT14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:280" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update documents, references and user guide.
</commit_message>
<xml_diff>
--- a/downloads/DRAC_Input_and_Output_Template.xlsx
+++ b/downloads/DRAC_Input_and_Output_Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DRAC_1.1_input" sheetId="1" r:id="rId1"/>
@@ -969,32 +969,6 @@
   </si>
   <si>
     <t>Th Alpha grain size absorption factor</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Please cite all uses of DRAC, including the version number, as Durcan, J.A., King, G.E., and Duller, G.A.T., 2015. DRAC: Dose rate and age calculator for trapped charge dating. Quaternary Geochronology, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>XX, XX-XX</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Corresponding authors: Julie Durcan (julie.durcan@ouce.ox.ac.uk) and Georgina King (georgina.king@unil.ch).</t>
-    </r>
   </si>
   <si>
     <t>DRAC-example</t>
@@ -1708,7 +1682,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Full details of the inputs required for a DRAC dose rate calculation and the calculation process can be found in the paper </t>
+      <t xml:space="preserve">Please cite all uses of DRAC, including the version number, as Durcan, J.A., King, G.E., and Duller, G.A.T., 2015. DRAC: Dose rate and age calculator for trapped charge dating. Quaternary Geochronology, </t>
     </r>
     <r>
       <rPr>
@@ -1719,7 +1693,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>XXXX</t>
+      <t>28, 54-61</t>
     </r>
     <r>
       <rPr>
@@ -1729,7 +1703,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> and the DRAC website </t>
+      <t>. Corresponding authors: Julie Durcan (julie.durcan@ouce.ox.ac.uk) and Georgina King (georgina.king@unil.ch).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Full details of the inputs required for a DRAC dose rate calculation and the calculation process can be found in the paper by Durcan et al. (2015) and the DRAC website </t>
     </r>
     <r>
       <rPr>
@@ -2191,8 +2170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2269,12 +2248,12 @@
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>318</v>
+        <v>547</v>
       </c>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.25">
@@ -2455,25 +2434,25 @@
         <v>8</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>20</v>
@@ -2482,100 +2461,100 @@
         <v>22</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>25</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="R11" s="6" t="s">
         <v>28</v>
       </c>
       <c r="S11" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="T11" s="6" t="s">
         <v>31</v>
       </c>
       <c r="U11" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="V11" s="6" t="s">
         <v>34</v>
       </c>
       <c r="W11" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="X11" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="Y11" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="X11" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="Y11" s="6" t="s">
+      <c r="Z11" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="AA11" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="Z11" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="AA11" s="6" t="s">
+      <c r="AB11" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="AC11" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="AB11" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="AC11" s="6" t="s">
+      <c r="AD11" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="AE11" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="AD11" s="6" t="s">
-        <v>353</v>
-      </c>
-      <c r="AE11" s="6" t="s">
+      <c r="AF11" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="AF11" s="6" t="s">
+      <c r="AG11" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="AG11" s="6" t="s">
+      <c r="AH11" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="AH11" s="6" t="s">
+      <c r="AI11" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="AI11" s="6" t="s">
+      <c r="AJ11" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="AJ11" s="6" t="s">
+      <c r="AK11" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="AK11" s="6" t="s">
+      <c r="AL11" s="6" t="s">
         <v>344</v>
-      </c>
-      <c r="AL11" s="6" t="s">
-        <v>345</v>
       </c>
       <c r="AM11" s="6" t="s">
         <v>50</v>
       </c>
       <c r="AN11" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AO11" s="6" t="s">
         <v>53</v>
       </c>
       <c r="AP11" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AQ11" s="6" t="s">
         <v>56</v>
       </c>
       <c r="AR11" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AS11" s="6" t="s">
         <v>59</v>
       </c>
       <c r="AT11" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AU11" s="6" t="s">
         <v>62</v>
@@ -2587,30 +2566,30 @@
         <v>66</v>
       </c>
       <c r="AX11" s="6" t="s">
+        <v>346</v>
+      </c>
+      <c r="AY11" s="6" t="s">
         <v>347</v>
-      </c>
-      <c r="AY11" s="6" t="s">
-        <v>348</v>
       </c>
       <c r="AZ11" s="6" t="s">
         <v>70</v>
       </c>
       <c r="BA11" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>319</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="C12" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="D12" s="17" t="s">
         <v>321</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>322</v>
       </c>
       <c r="E12" s="17">
         <v>3.4</v>
@@ -2637,61 +2616,61 @@
         <v>0</v>
       </c>
       <c r="M12" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="N12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="O12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="P12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Q12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="R12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="S12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="T12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="U12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="V12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="W12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="X12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Y12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Z12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AA12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AB12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AC12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AD12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AE12" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AF12" s="17">
         <v>90</v>
@@ -2700,10 +2679,10 @@
         <v>125</v>
       </c>
       <c r="AH12" s="17" t="s">
+        <v>323</v>
+      </c>
+      <c r="AI12" s="17" t="s">
         <v>324</v>
-      </c>
-      <c r="AI12" s="17" t="s">
-        <v>325</v>
       </c>
       <c r="AJ12" s="17">
         <v>8</v>
@@ -2712,7 +2691,7 @@
         <v>10</v>
       </c>
       <c r="AL12" s="17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AM12" s="17">
         <v>0</v>
@@ -2748,10 +2727,10 @@
         <v>150</v>
       </c>
       <c r="AX12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AY12" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AZ12" s="17">
         <v>20</v>
@@ -2762,16 +2741,16 @@
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>285</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E13" s="17">
         <v>2</v>
@@ -2798,19 +2777,19 @@
         <v>0</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="N13" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="O13" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="P13" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Q13" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="R13" s="17">
         <v>12.5</v>
@@ -2819,40 +2798,40 @@
         <v>0.5</v>
       </c>
       <c r="T13" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="U13" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="V13" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="W13" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="X13" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Y13" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Z13" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AA13" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AB13" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AC13" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AD13" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AE13" s="17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AF13" s="17">
         <v>180</v>
@@ -2861,10 +2840,10 @@
         <v>212</v>
       </c>
       <c r="AH13" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="AI13" s="17" t="s">
         <v>329</v>
-      </c>
-      <c r="AI13" s="17" t="s">
-        <v>330</v>
       </c>
       <c r="AJ13" s="17">
         <v>0</v>
@@ -2873,7 +2852,7 @@
         <v>0</v>
       </c>
       <c r="AL13" s="17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AM13" s="17">
         <v>0.15</v>
@@ -2909,10 +2888,10 @@
         <v>200</v>
       </c>
       <c r="AX13" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AY13" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AZ13" s="17">
         <v>15</v>
@@ -2923,16 +2902,16 @@
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B14" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>331</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>332</v>
-      </c>
       <c r="D14" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E14" s="17">
         <v>4</v>
@@ -2959,19 +2938,19 @@
         <v>0</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="O14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="P14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Q14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="R14" s="17">
         <v>12.5</v>
@@ -2980,19 +2959,19 @@
         <v>0.5</v>
       </c>
       <c r="T14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="U14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="V14" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="W14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="X14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Y14" s="17">
         <v>2.5</v>
@@ -3001,19 +2980,19 @@
         <v>0.15</v>
       </c>
       <c r="AA14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AB14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AC14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AD14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AE14" s="17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AF14" s="17">
         <v>4</v>
@@ -3022,10 +3001,10 @@
         <v>11</v>
       </c>
       <c r="AH14" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="AI14" s="17" t="s">
         <v>329</v>
-      </c>
-      <c r="AI14" s="17" t="s">
-        <v>330</v>
       </c>
       <c r="AJ14" s="17">
         <v>0</v>
@@ -3034,7 +3013,7 @@
         <v>0</v>
       </c>
       <c r="AL14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AM14" s="17">
         <v>8.5999999999999993E-2</v>
@@ -3049,25 +3028,25 @@
         <v>5</v>
       </c>
       <c r="AQ14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AR14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AS14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AT14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AU14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AV14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AW14" s="17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AX14" s="17">
         <v>0.2</v>
@@ -3091,8 +3070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:JT277"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3390,7 +3369,7 @@
     </row>
     <row r="6" spans="1:280" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>318</v>
+        <v>547</v>
       </c>
     </row>
     <row r="8" spans="1:280" x14ac:dyDescent="0.25">
@@ -4255,70 +4234,70 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
+        <v>364</v>
+      </c>
+      <c r="E14" t="s">
         <v>365</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>366</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>367</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>368</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>369</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>370</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>371</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>372</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>373</v>
-      </c>
-      <c r="M14" t="s">
-        <v>374</v>
       </c>
       <c r="N14" t="s">
         <v>288</v>
       </c>
       <c r="O14" t="s">
+        <v>374</v>
+      </c>
+      <c r="P14" t="s">
         <v>375</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>376</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>377</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>378</v>
-      </c>
-      <c r="S14" t="s">
-        <v>379</v>
       </c>
       <c r="T14" t="s">
         <v>310</v>
       </c>
       <c r="U14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="V14" t="s">
         <v>70</v>
       </c>
       <c r="W14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="X14" t="s">
         <v>292</v>
       </c>
       <c r="Y14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AB14" s="12" t="s">
         <v>306</v>
@@ -4336,25 +4315,25 @@
         <v>8</v>
       </c>
       <c r="AG14" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AH14" s="14" t="s">
         <v>11</v>
       </c>
       <c r="AI14" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AJ14" s="14" t="s">
         <v>14</v>
       </c>
       <c r="AK14" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AL14" s="14" t="s">
         <v>17</v>
       </c>
       <c r="AM14" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="AN14" s="14" t="s">
         <v>20</v>
@@ -4363,100 +4342,100 @@
         <v>22</v>
       </c>
       <c r="AP14" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AQ14" s="14" t="s">
         <v>25</v>
       </c>
       <c r="AR14" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AS14" s="14" t="s">
         <v>28</v>
       </c>
       <c r="AT14" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AU14" s="14" t="s">
         <v>31</v>
       </c>
       <c r="AV14" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AW14" s="14" t="s">
         <v>34</v>
       </c>
       <c r="AX14" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="AY14" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="AZ14" s="14" t="s">
         <v>334</v>
       </c>
-      <c r="AY14" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="AZ14" s="14" t="s">
+      <c r="BA14" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="BB14" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="BA14" s="14" t="s">
-        <v>355</v>
-      </c>
-      <c r="BB14" s="14" t="s">
+      <c r="BC14" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="BD14" s="14" t="s">
         <v>336</v>
       </c>
-      <c r="BC14" s="14" t="s">
-        <v>354</v>
-      </c>
-      <c r="BD14" s="14" t="s">
+      <c r="BE14" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="BF14" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="BE14" s="14" t="s">
-        <v>353</v>
-      </c>
-      <c r="BF14" s="14" t="s">
+      <c r="BG14" s="14" t="s">
         <v>338</v>
       </c>
-      <c r="BG14" s="14" t="s">
+      <c r="BH14" s="14" t="s">
         <v>339</v>
       </c>
-      <c r="BH14" s="14" t="s">
+      <c r="BI14" s="14" t="s">
         <v>340</v>
       </c>
-      <c r="BI14" s="14" t="s">
+      <c r="BJ14" s="14" t="s">
         <v>341</v>
       </c>
-      <c r="BJ14" s="14" t="s">
+      <c r="BK14" s="14" t="s">
         <v>342</v>
       </c>
-      <c r="BK14" s="14" t="s">
+      <c r="BL14" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="BL14" s="14" t="s">
+      <c r="BM14" s="14" t="s">
         <v>344</v>
-      </c>
-      <c r="BM14" s="14" t="s">
-        <v>345</v>
       </c>
       <c r="BN14" s="14" t="s">
         <v>50</v>
       </c>
       <c r="BO14" s="14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="BP14" s="14" t="s">
         <v>53</v>
       </c>
       <c r="BQ14" s="14" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="BR14" s="14" t="s">
         <v>56</v>
       </c>
       <c r="BS14" s="14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="BT14" s="14" t="s">
         <v>59</v>
       </c>
       <c r="BU14" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="BV14" s="14" t="s">
         <v>62</v>
@@ -4468,569 +4447,569 @@
         <v>66</v>
       </c>
       <c r="BY14" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="BZ14" s="14" t="s">
         <v>347</v>
-      </c>
-      <c r="BZ14" s="14" t="s">
-        <v>348</v>
       </c>
       <c r="CA14" s="14" t="s">
         <v>70</v>
       </c>
       <c r="CB14" s="14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="CC14" s="11"/>
       <c r="CE14" t="s">
+        <v>381</v>
+      </c>
+      <c r="CF14" t="s">
         <v>382</v>
       </c>
-      <c r="CF14" t="s">
+      <c r="CG14" t="s">
         <v>383</v>
       </c>
-      <c r="CG14" t="s">
+      <c r="CH14" t="s">
         <v>384</v>
       </c>
-      <c r="CH14" t="s">
+      <c r="CI14" t="s">
         <v>385</v>
       </c>
-      <c r="CI14" t="s">
+      <c r="CJ14" t="s">
         <v>386</v>
       </c>
-      <c r="CJ14" t="s">
+      <c r="CK14" t="s">
         <v>387</v>
       </c>
-      <c r="CK14" t="s">
+      <c r="CL14" t="s">
         <v>388</v>
       </c>
-      <c r="CL14" t="s">
+      <c r="CM14" t="s">
         <v>389</v>
       </c>
-      <c r="CM14" t="s">
+      <c r="CN14" t="s">
         <v>390</v>
       </c>
-      <c r="CN14" t="s">
+      <c r="CO14" t="s">
         <v>391</v>
       </c>
-      <c r="CO14" t="s">
+      <c r="CP14" t="s">
         <v>392</v>
       </c>
-      <c r="CP14" t="s">
+      <c r="CQ14" t="s">
         <v>393</v>
       </c>
-      <c r="CQ14" t="s">
+      <c r="CR14" t="s">
         <v>394</v>
       </c>
-      <c r="CR14" t="s">
+      <c r="CS14" t="s">
         <v>395</v>
       </c>
-      <c r="CS14" t="s">
+      <c r="CT14" t="s">
         <v>396</v>
       </c>
-      <c r="CT14" t="s">
+      <c r="CU14" t="s">
         <v>397</v>
       </c>
-      <c r="CU14" t="s">
+      <c r="CV14" t="s">
         <v>398</v>
       </c>
-      <c r="CV14" t="s">
+      <c r="CW14" t="s">
         <v>399</v>
       </c>
-      <c r="CW14" t="s">
+      <c r="CX14" t="s">
         <v>400</v>
       </c>
-      <c r="CX14" t="s">
+      <c r="CY14" t="s">
         <v>401</v>
       </c>
-      <c r="CY14" t="s">
+      <c r="CZ14" t="s">
         <v>402</v>
       </c>
-      <c r="CZ14" t="s">
+      <c r="DA14" t="s">
         <v>403</v>
       </c>
-      <c r="DA14" t="s">
+      <c r="DB14" t="s">
         <v>404</v>
       </c>
-      <c r="DB14" t="s">
+      <c r="DC14" t="s">
         <v>405</v>
       </c>
-      <c r="DC14" t="s">
+      <c r="DD14" t="s">
         <v>406</v>
       </c>
-      <c r="DD14" t="s">
+      <c r="DE14" t="s">
+        <v>408</v>
+      </c>
+      <c r="DF14" s="15" t="s">
         <v>407</v>
       </c>
-      <c r="DE14" t="s">
+      <c r="DG14" t="s">
         <v>409</v>
       </c>
-      <c r="DF14" s="15" t="s">
-        <v>408</v>
-      </c>
-      <c r="DG14" t="s">
+      <c r="DH14" t="s">
         <v>410</v>
       </c>
-      <c r="DH14" t="s">
+      <c r="DI14" t="s">
         <v>411</v>
       </c>
-      <c r="DI14" t="s">
+      <c r="DJ14" t="s">
         <v>412</v>
       </c>
-      <c r="DJ14" t="s">
+      <c r="DK14" t="s">
         <v>413</v>
       </c>
-      <c r="DK14" t="s">
+      <c r="DL14" t="s">
         <v>414</v>
       </c>
-      <c r="DL14" t="s">
+      <c r="DM14" t="s">
         <v>415</v>
       </c>
-      <c r="DM14" t="s">
+      <c r="DN14" t="s">
         <v>416</v>
       </c>
-      <c r="DN14" t="s">
+      <c r="DO14" t="s">
         <v>417</v>
       </c>
-      <c r="DO14" t="s">
+      <c r="DP14" t="s">
         <v>418</v>
       </c>
-      <c r="DP14" t="s">
+      <c r="DQ14" t="s">
         <v>419</v>
       </c>
-      <c r="DQ14" t="s">
+      <c r="DR14" t="s">
         <v>420</v>
       </c>
-      <c r="DR14" t="s">
+      <c r="DS14" t="s">
         <v>421</v>
       </c>
-      <c r="DS14" t="s">
+      <c r="DT14" t="s">
         <v>422</v>
       </c>
-      <c r="DT14" t="s">
+      <c r="DU14" t="s">
         <v>423</v>
       </c>
-      <c r="DU14" t="s">
+      <c r="DV14" t="s">
         <v>424</v>
       </c>
-      <c r="DV14" t="s">
+      <c r="DW14" t="s">
         <v>425</v>
       </c>
-      <c r="DW14" t="s">
+      <c r="DX14" t="s">
         <v>426</v>
       </c>
-      <c r="DX14" t="s">
+      <c r="DY14" t="s">
         <v>427</v>
       </c>
-      <c r="DY14" t="s">
+      <c r="DZ14" t="s">
         <v>428</v>
       </c>
-      <c r="DZ14" t="s">
+      <c r="EA14" t="s">
         <v>429</v>
       </c>
-      <c r="EA14" t="s">
+      <c r="EB14" t="s">
         <v>430</v>
       </c>
-      <c r="EB14" t="s">
+      <c r="EC14" t="s">
         <v>431</v>
       </c>
-      <c r="EC14" t="s">
+      <c r="ED14" t="s">
         <v>432</v>
-      </c>
-      <c r="ED14" t="s">
-        <v>433</v>
       </c>
       <c r="EE14" t="s">
         <v>313</v>
       </c>
       <c r="EF14" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="EG14" t="s">
         <v>314</v>
       </c>
       <c r="EH14" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="EI14" t="s">
         <v>315</v>
       </c>
       <c r="EJ14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="EK14" t="s">
         <v>316</v>
       </c>
       <c r="EL14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="EM14" t="s">
         <v>317</v>
       </c>
       <c r="EN14" t="s">
+        <v>436</v>
+      </c>
+      <c r="EO14" t="s">
         <v>437</v>
       </c>
-      <c r="EO14" t="s">
+      <c r="EP14" t="s">
         <v>438</v>
       </c>
-      <c r="EP14" t="s">
+      <c r="EQ14" t="s">
         <v>439</v>
       </c>
-      <c r="EQ14" t="s">
+      <c r="ER14" t="s">
         <v>440</v>
       </c>
-      <c r="ER14" t="s">
+      <c r="ES14" t="s">
         <v>441</v>
       </c>
-      <c r="ES14" t="s">
+      <c r="ET14" t="s">
         <v>442</v>
       </c>
-      <c r="ET14" t="s">
+      <c r="EU14" t="s">
         <v>443</v>
       </c>
-      <c r="EU14" t="s">
+      <c r="EV14" t="s">
         <v>444</v>
       </c>
-      <c r="EV14" t="s">
+      <c r="EW14" t="s">
         <v>445</v>
       </c>
-      <c r="EW14" t="s">
+      <c r="EX14" t="s">
         <v>446</v>
-      </c>
-      <c r="EX14" t="s">
-        <v>447</v>
       </c>
       <c r="EY14" t="s">
         <v>263</v>
       </c>
       <c r="EZ14" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="FA14" t="s">
         <v>264</v>
       </c>
       <c r="FB14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="FC14" t="s">
         <v>265</v>
       </c>
       <c r="FD14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="FE14" t="s">
         <v>266</v>
       </c>
       <c r="FF14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="FG14" t="s">
         <v>267</v>
       </c>
       <c r="FH14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="FI14" t="s">
         <v>268</v>
       </c>
       <c r="FJ14" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="FK14" t="s">
         <v>269</v>
       </c>
       <c r="FL14" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="FM14" t="s">
         <v>270</v>
       </c>
       <c r="FN14" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="FO14" t="s">
         <v>271</v>
       </c>
       <c r="FP14" t="s">
+        <v>455</v>
+      </c>
+      <c r="FQ14" t="s">
         <v>456</v>
       </c>
-      <c r="FQ14" t="s">
+      <c r="FR14" t="s">
         <v>457</v>
       </c>
-      <c r="FR14" t="s">
+      <c r="FS14" t="s">
         <v>458</v>
       </c>
-      <c r="FS14" t="s">
+      <c r="FT14" t="s">
         <v>459</v>
       </c>
-      <c r="FT14" t="s">
+      <c r="FU14" t="s">
         <v>460</v>
       </c>
-      <c r="FU14" t="s">
+      <c r="FV14" t="s">
         <v>461</v>
       </c>
-      <c r="FV14" t="s">
+      <c r="FW14" t="s">
         <v>462</v>
       </c>
-      <c r="FW14" t="s">
+      <c r="FX14" t="s">
         <v>463</v>
       </c>
-      <c r="FX14" t="s">
+      <c r="FY14" t="s">
         <v>464</v>
       </c>
-      <c r="FY14" t="s">
+      <c r="FZ14" t="s">
         <v>465</v>
       </c>
-      <c r="FZ14" t="s">
+      <c r="GA14" t="s">
         <v>466</v>
       </c>
-      <c r="GA14" t="s">
+      <c r="GB14" t="s">
         <v>467</v>
       </c>
-      <c r="GB14" t="s">
+      <c r="GC14" t="s">
         <v>468</v>
       </c>
-      <c r="GC14" t="s">
+      <c r="GD14" t="s">
         <v>469</v>
       </c>
-      <c r="GD14" t="s">
+      <c r="GE14" t="s">
         <v>470</v>
       </c>
-      <c r="GE14" t="s">
+      <c r="GF14" t="s">
         <v>471</v>
       </c>
-      <c r="GF14" t="s">
+      <c r="GG14" t="s">
         <v>472</v>
       </c>
-      <c r="GG14" t="s">
+      <c r="GH14" t="s">
         <v>473</v>
-      </c>
-      <c r="GH14" t="s">
-        <v>474</v>
       </c>
       <c r="GI14" t="s">
         <v>272</v>
       </c>
       <c r="GJ14" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="GK14" t="s">
         <v>273</v>
       </c>
       <c r="GL14" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="GM14" t="s">
         <v>274</v>
       </c>
       <c r="GN14" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="GO14" t="s">
         <v>275</v>
       </c>
       <c r="GP14" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="GQ14" t="s">
         <v>276</v>
       </c>
       <c r="GR14" t="s">
+        <v>478</v>
+      </c>
+      <c r="GS14" t="s">
         <v>479</v>
       </c>
-      <c r="GS14" t="s">
+      <c r="GT14" t="s">
         <v>480</v>
       </c>
-      <c r="GT14" t="s">
+      <c r="GU14" t="s">
         <v>481</v>
       </c>
-      <c r="GU14" t="s">
+      <c r="GV14" t="s">
         <v>482</v>
       </c>
-      <c r="GV14" t="s">
+      <c r="GW14" t="s">
         <v>483</v>
       </c>
-      <c r="GW14" t="s">
+      <c r="GX14" t="s">
         <v>484</v>
       </c>
-      <c r="GX14" t="s">
+      <c r="GY14" t="s">
         <v>485</v>
       </c>
-      <c r="GY14" t="s">
+      <c r="GZ14" t="s">
         <v>486</v>
       </c>
-      <c r="GZ14" t="s">
+      <c r="HA14" t="s">
         <v>487</v>
       </c>
-      <c r="HA14" t="s">
+      <c r="HB14" t="s">
         <v>488</v>
-      </c>
-      <c r="HB14" t="s">
-        <v>489</v>
       </c>
       <c r="HC14" t="s">
         <v>277</v>
       </c>
       <c r="HD14" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="HE14" t="s">
         <v>278</v>
       </c>
       <c r="HF14" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="HG14" t="s">
         <v>279</v>
       </c>
       <c r="HH14" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="HI14" t="s">
         <v>280</v>
       </c>
       <c r="HJ14" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="HK14" t="s">
         <v>281</v>
       </c>
       <c r="HL14" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="HM14" t="s">
         <v>282</v>
       </c>
       <c r="HN14" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="HO14" t="s">
         <v>283</v>
       </c>
       <c r="HP14" t="s">
+        <v>495</v>
+      </c>
+      <c r="HQ14" t="s">
         <v>496</v>
       </c>
-      <c r="HQ14" t="s">
+      <c r="HR14" t="s">
         <v>497</v>
       </c>
-      <c r="HR14" t="s">
+      <c r="HS14" t="s">
         <v>498</v>
       </c>
-      <c r="HS14" t="s">
+      <c r="HT14" t="s">
         <v>499</v>
       </c>
-      <c r="HT14" t="s">
+      <c r="HU14" t="s">
         <v>500</v>
       </c>
-      <c r="HU14" t="s">
+      <c r="HV14" t="s">
         <v>501</v>
       </c>
-      <c r="HV14" t="s">
+      <c r="HW14" t="s">
         <v>502</v>
       </c>
-      <c r="HW14" t="s">
+      <c r="HX14" t="s">
         <v>503</v>
       </c>
-      <c r="HX14" t="s">
+      <c r="HY14" t="s">
         <v>504</v>
       </c>
-      <c r="HY14" t="s">
+      <c r="HZ14" t="s">
         <v>505</v>
       </c>
-      <c r="HZ14" t="s">
+      <c r="IA14" t="s">
         <v>506</v>
       </c>
-      <c r="IA14" t="s">
+      <c r="IB14" t="s">
         <v>507</v>
       </c>
-      <c r="IB14" t="s">
+      <c r="IC14" t="s">
         <v>508</v>
       </c>
-      <c r="IC14" t="s">
+      <c r="ID14" t="s">
         <v>509</v>
       </c>
-      <c r="ID14" t="s">
+      <c r="IE14" t="s">
         <v>510</v>
       </c>
-      <c r="IE14" t="s">
+      <c r="IF14" t="s">
         <v>511</v>
       </c>
-      <c r="IF14" t="s">
+      <c r="IG14" t="s">
         <v>512</v>
       </c>
-      <c r="IG14" t="s">
+      <c r="IH14" t="s">
         <v>513</v>
       </c>
-      <c r="IH14" t="s">
+      <c r="II14" t="s">
         <v>514</v>
       </c>
-      <c r="II14" t="s">
+      <c r="IJ14" t="s">
         <v>515</v>
       </c>
-      <c r="IJ14" t="s">
+      <c r="IK14" t="s">
         <v>516</v>
       </c>
-      <c r="IK14" t="s">
+      <c r="IL14" t="s">
         <v>517</v>
       </c>
-      <c r="IL14" t="s">
+      <c r="IM14" t="s">
         <v>518</v>
       </c>
-      <c r="IM14" t="s">
+      <c r="IN14" t="s">
         <v>519</v>
       </c>
-      <c r="IN14" t="s">
+      <c r="IO14" t="s">
         <v>520</v>
       </c>
-      <c r="IO14" t="s">
+      <c r="IP14" t="s">
         <v>521</v>
       </c>
-      <c r="IP14" t="s">
+      <c r="IQ14" t="s">
         <v>522</v>
       </c>
-      <c r="IQ14" t="s">
+      <c r="IR14" t="s">
         <v>523</v>
       </c>
-      <c r="IR14" t="s">
+      <c r="IS14" t="s">
         <v>524</v>
       </c>
-      <c r="IS14" t="s">
+      <c r="IT14" t="s">
         <v>525</v>
       </c>
-      <c r="IT14" t="s">
+      <c r="IU14" t="s">
         <v>526</v>
       </c>
-      <c r="IU14" t="s">
+      <c r="IV14" t="s">
         <v>527</v>
       </c>
-      <c r="IV14" t="s">
+      <c r="IW14" t="s">
         <v>528</v>
       </c>
-      <c r="IW14" t="s">
+      <c r="IX14" t="s">
         <v>529</v>
       </c>
-      <c r="IX14" t="s">
+      <c r="IY14" t="s">
         <v>530</v>
       </c>
-      <c r="IY14" t="s">
+      <c r="IZ14" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="IZ14" s="4" t="s">
+      <c r="JA14" t="s">
         <v>532</v>
       </c>
-      <c r="JA14" t="s">
+      <c r="JB14" t="s">
         <v>533</v>
       </c>
-      <c r="JB14" t="s">
+      <c r="JC14" t="s">
         <v>534</v>
       </c>
-      <c r="JC14" t="s">
+      <c r="JD14" t="s">
         <v>535</v>
       </c>
-      <c r="JD14" t="s">
+      <c r="JE14" t="s">
         <v>536</v>
       </c>
-      <c r="JE14" t="s">
+      <c r="JF14" t="s">
         <v>537</v>
-      </c>
-      <c r="JF14" t="s">
-        <v>538</v>
       </c>
       <c r="JG14" t="s">
         <v>284</v>
@@ -5045,34 +5024,34 @@
         <v>287</v>
       </c>
       <c r="JK14" t="s">
+        <v>538</v>
+      </c>
+      <c r="JL14" t="s">
         <v>539</v>
       </c>
-      <c r="JL14" t="s">
+      <c r="JM14" t="s">
         <v>540</v>
       </c>
-      <c r="JM14" t="s">
+      <c r="JN14" t="s">
         <v>541</v>
       </c>
-      <c r="JN14" t="s">
+      <c r="JO14" t="s">
         <v>542</v>
       </c>
-      <c r="JO14" t="s">
+      <c r="JP14" t="s">
         <v>543</v>
-      </c>
-      <c r="JP14" t="s">
-        <v>544</v>
       </c>
       <c r="JQ14" t="s">
         <v>289</v>
       </c>
       <c r="JR14" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="JS14" t="s">
         <v>292</v>
       </c>
       <c r="JT14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="1:280" x14ac:dyDescent="0.25">

</xml_diff>